<commit_message>
second commit from pradnya
</commit_message>
<xml_diff>
--- a/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
+++ b/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
@@ -415,27 +415,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -459,12 +438,39 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -472,12 +478,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -753,7 +753,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -778,118 +778,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -979,6 +979,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:F7"/>
@@ -992,12 +998,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" activeCellId="1" sqref="A16 A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,114 +1040,114 @@
         <v>0</v>
       </c>
       <c r="B5" s="26"/>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="26"/>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="26"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="26"/>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="26"/>
-      <c r="C9" s="30">
+      <c r="C9" s="27">
         <v>44379</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="31">
+      <c r="B10" s="19"/>
+      <c r="C10" s="28">
         <v>44379</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1176,7 +1176,7 @@
       <c r="B16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -1228,10 +1228,10 @@
       <c r="B20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="10" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="5"/>
@@ -1259,28 +1259,28 @@
     </row>
     <row r="23" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="11" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="16"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="6"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1290,111 +1290,111 @@
         <v>0</v>
       </c>
       <c r="B26" s="26"/>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="22"/>
     </row>
     <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="26"/>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="31"/>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="15"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B29" s="26"/>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="15"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="22"/>
     </row>
     <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="26"/>
-      <c r="C30" s="30">
+      <c r="C30" s="27">
         <v>44379</v>
       </c>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="15"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="31">
+      <c r="B31" s="19"/>
+      <c r="C31" s="28">
         <v>44379</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="13" t="s">
+      <c r="B32" s="19"/>
+      <c r="C32" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="15"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10" t="s">
+      <c r="B33" s="19"/>
+      <c r="C33" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="10" t="s">
+      <c r="B34" s="19"/>
+      <c r="C34" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
-      <c r="C35" s="16"/>
+      <c r="C35" s="9"/>
       <c r="D35" s="6"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="20"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -1468,12 +1468,12 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
     </row>
     <row r="44" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
@@ -1482,7 +1482,7 @@
       <c r="B44" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D44" s="6" t="s">
@@ -1543,7 +1543,7 @@
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="5"/>
@@ -1566,27 +1566,54 @@
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="21"/>
-      <c r="B51" s="22" t="s">
+      <c r="A51" s="14"/>
+      <c r="B51" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="21"/>
-      <c r="D51" s="23" t="s">
+      <c r="C51" s="14"/>
+      <c r="D51" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:F29"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="C33:F33"/>
     <mergeCell ref="A34:B34"/>
@@ -1597,33 +1624,6 @@
     <mergeCell ref="C31:F31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="C32:F32"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update the Manual testcases
</commit_message>
<xml_diff>
--- a/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
+++ b/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067CBF29-336E-4CC3-BC62-0E1012DFC232}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="167" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
   <si>
     <t>Project Name:</t>
   </si>
@@ -88,13 +89,106 @@
   </si>
   <si>
     <t>SCENARIO DESCRIPTION</t>
+  </si>
+  <si>
+    <t>click on credit module  ,click on status textfield select active and click on Enter credit fill the details and click on save</t>
+  </si>
+  <si>
+    <t>client account should be created</t>
+  </si>
+  <si>
+    <t>credis should be created</t>
+  </si>
+  <si>
+    <t>click on status textfield select active and check the  client name box and click on select and click on edit credit and edit the information and save</t>
+  </si>
+  <si>
+    <t>credits should be created</t>
+  </si>
+  <si>
+    <t>click on select dropdown select apply credit and fill the information and click on save</t>
+  </si>
+  <si>
+    <t>client account should be createdcredits should be created</t>
+  </si>
+  <si>
+    <t>https://app.invoiceninja.com/</t>
+  </si>
+  <si>
+    <t>Enter the valid data and click on 'Login' button</t>
+  </si>
+  <si>
+    <t>un:sowmya h m, password:Hithuma@12345</t>
+  </si>
+  <si>
+    <t>Login' Page should be displayed</t>
+  </si>
+  <si>
+    <t>Home'page is displayed</t>
+  </si>
+  <si>
+    <t>click on 'Credits' module</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Credits page is displayed</t>
+  </si>
+  <si>
+    <t>click on 'Enter Credit'  Button</t>
+  </si>
+  <si>
+    <t>enter credit page is displayed</t>
+  </si>
+  <si>
+    <t>client name:sowmya h m</t>
+  </si>
+  <si>
+    <t>status: active</t>
+  </si>
+  <si>
+    <t>selected active status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click on select dropdown </t>
+  </si>
+  <si>
+    <t>display all option</t>
+  </si>
+  <si>
+    <t>click on edit credit and edit the information  and  click on save</t>
+  </si>
+  <si>
+    <t>save the information</t>
+  </si>
+  <si>
+    <t>TC2 1</t>
+  </si>
+  <si>
+    <t>Enter all valid data and click on 'Save'  Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> click on 'Logout' Button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">click on 'Status' dropdown </t>
+  </si>
+  <si>
+    <t>Open the application enter the  test Url</t>
+  </si>
+  <si>
+    <t>logged out successfully</t>
+  </si>
+  <si>
+    <t>click on 'Logout' Button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +229,14 @@
       <color rgb="FFFFFFFF"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -218,10 +320,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -238,6 +341,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -254,19 +366,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,17 +654,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="73" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="32.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="31.140625" style="1" customWidth="1"/>
@@ -562,114 +672,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -692,25 +802,47 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="5">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="A13" s="5">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="A14" s="5">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -749,12 +881,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:F7"/>
@@ -768,6 +894,12 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -775,7 +907,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -789,7 +921,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
@@ -803,7 +935,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -815,7 +947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -827,7 +959,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -839,7 +971,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -851,19 +983,494 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="70.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{9F56FFCA-70B0-4140-AB4E-8A211C87CE1E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -875,7 +1482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
updated the manual test cases
</commit_message>
<xml_diff>
--- a/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
+++ b/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067CBF29-336E-4CC3-BC62-0E1012DFC232}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93652384-1234-419C-88A1-3E245F90F63A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="167" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
   <si>
     <t>Project Name:</t>
   </si>
@@ -124,24 +124,15 @@
     <t>Login' Page should be displayed</t>
   </si>
   <si>
-    <t>Home'page is displayed</t>
-  </si>
-  <si>
     <t>click on 'Credits' module</t>
   </si>
   <si>
     <t>NA</t>
   </si>
   <si>
-    <t>Credits page is displayed</t>
-  </si>
-  <si>
     <t>click on 'Enter Credit'  Button</t>
   </si>
   <si>
-    <t>enter credit page is displayed</t>
-  </si>
-  <si>
     <t>client name:sowmya h m</t>
   </si>
   <si>
@@ -163,9 +154,6 @@
     <t>save the information</t>
   </si>
   <si>
-    <t>TC2 1</t>
-  </si>
-  <si>
     <t>Enter all valid data and click on 'Save'  Button</t>
   </si>
   <si>
@@ -182,6 +170,24 @@
   </si>
   <si>
     <t>click on 'Logout' Button</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>Tc_02</t>
+  </si>
+  <si>
+    <t>Home'page  should be displayed</t>
+  </si>
+  <si>
+    <t>Credits page should bedisplayed</t>
+  </si>
+  <si>
+    <t>enter credit page should be displayed</t>
+  </si>
+  <si>
+    <t>Home'page should be displayed</t>
   </si>
 </sst>
 </file>
@@ -324,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -341,37 +347,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -672,114 +681,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -881,6 +890,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:F7"/>
@@ -894,12 +909,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -986,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,122 +1009,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1138,16 +1147,16 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>1</v>
+      <c r="A13" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E13" s="5"/>
@@ -1161,8 +1170,8 @@
       <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="16" t="s">
-        <v>31</v>
+      <c r="D14" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1172,13 +1181,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -1188,13 +1197,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1204,10 +1213,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>24</v>
@@ -1220,94 +1229,98 @@
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>41</v>
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="A21" s="17">
+        <v>2</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>43</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>4</v>
+      <c r="A22" s="17">
+        <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="A23" s="17">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="A24" s="1">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
@@ -1441,6 +1454,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A7:B7"/>
@@ -1449,18 +1474,6 @@
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C13" r:id="rId1" xr:uid="{9F56FFCA-70B0-4140-AB4E-8A211C87CE1E}"/>

</xml_diff>

<commit_message>
sending new test case projects module
</commit_message>
<xml_diff>
--- a/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
+++ b/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11310" windowHeight="4035"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Tasks" sheetId="9" r:id="rId9"/>
     <sheet name="Vendors" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:H19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -93,7 +94,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -325,7 +326,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -360,7 +361,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -537,7 +538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,7 +549,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +794,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:B26"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Manual test case (Credits)
</commit_message>
<xml_diff>
--- a/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
+++ b/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Tasks" sheetId="9" r:id="rId9"/>
     <sheet name="Vendors" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="52">
   <si>
     <t>Project Name:</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Date of creation:</t>
   </si>
   <si>
-    <t>DD-MMM-YY</t>
-  </si>
-  <si>
     <t>Date of review:</t>
   </si>
   <si>
@@ -88,13 +85,112 @@
   </si>
   <si>
     <t>SCENARIO DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Navigate to the Application</t>
+  </si>
+  <si>
+    <t>https://app.invoiceninja.com/credits</t>
+  </si>
+  <si>
+    <t>Login page should be display</t>
+  </si>
+  <si>
+    <t>Login to the application</t>
+  </si>
+  <si>
+    <t>Username-valid, Password-valid</t>
+  </si>
+  <si>
+    <t>Home page should be display</t>
+  </si>
+  <si>
+    <t>Click on client button from left side dropdown</t>
+  </si>
+  <si>
+    <t>Clients page should be display</t>
+  </si>
+  <si>
+    <t>Click on new client button</t>
+  </si>
+  <si>
+    <t>Clients/Create page should be display</t>
+  </si>
+  <si>
+    <t>Enter valid information and click on SAVE button</t>
+  </si>
+  <si>
+    <t>Data- Valid</t>
+  </si>
+  <si>
+    <t>Should display the confirmation message as Client Successfully Created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on credits </t>
+  </si>
+  <si>
+    <t>Credits page should be display</t>
+  </si>
+  <si>
+    <t>Click on enter credit button</t>
+  </si>
+  <si>
+    <t>Credits/Create page should be display</t>
+  </si>
+  <si>
+    <t>Click on the dropdown arrow and select the client</t>
+  </si>
+  <si>
+    <t>Selected client should be displayed in the textfield</t>
+  </si>
+  <si>
+    <t>Enter valid data in all the textfields and click on SAVE button</t>
+  </si>
+  <si>
+    <t>Should display the confirmation message as Succesfully created credit</t>
+  </si>
+  <si>
+    <t>Click on the username icon in the upper right corner and click on logout</t>
+  </si>
+  <si>
+    <t>Shahbaj</t>
+  </si>
+  <si>
+    <t>TC_02CreditsTest</t>
+  </si>
+  <si>
+    <t>Username-Valid, Password-Valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on checkbox of any client </t>
+  </si>
+  <si>
+    <t>Checkbox should be selected</t>
+  </si>
+  <si>
+    <t>Click on select button and click on delete option from the opened dropdown</t>
+  </si>
+  <si>
+    <t>Should display the popup with popup message as are you sure</t>
+  </si>
+  <si>
+    <t>Click on OK</t>
+  </si>
+  <si>
+    <t>Should display the selected client successfully</t>
+  </si>
+  <si>
+    <t>Credits</t>
+  </si>
+  <si>
+    <t>TC_01CreditsTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +232,14 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -157,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -205,7 +309,129 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -213,33 +439,140 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -250,23 +583,104 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -545,216 +959,558 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="64.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="31.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="32"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="32"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="39">
+        <v>44379</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="32"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="39">
+        <v>44379</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="32"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="33"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="34"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="35"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="36"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38"/>
+    </row>
+    <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="B11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>1</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>2</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
         <v>3</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="11" t="s">
+      <c r="B14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
         <v>4</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="B15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>5</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>6</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>7</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>8</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>9</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
         <v>10</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="11" t="s">
+      <c r="B21" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="20"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="30"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="31"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="32"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="32"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="11" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" s="39">
+        <v>44379</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="32"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="39">
+        <v>44379</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="32"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="33"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="34"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="28"/>
+      <c r="C35" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="35"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="11" t="s">
+      <c r="D37" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>1</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>2</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>3</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>4</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="10"/>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>5</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="10"/>
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
         <v>6</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="B43" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="10"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="14">
+        <v>7</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="15"/>
+      <c r="F44" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
+  <mergeCells count="38">
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:F28"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:F7"/>
@@ -768,9 +1524,19 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C12" r:id="rId1"/>
+    <hyperlink ref="C38" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -852,12 +1618,620 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="65.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="32"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="32"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="39">
+        <v>44379</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="32"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="39">
+        <v>44379</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="32"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="33"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="34"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="35"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="36"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38"/>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>1</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>2</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>3</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>4</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>5</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>6</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>7</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>8</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>9</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
+        <v>10</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="30"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="31"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="32"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="32"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="39">
+        <v>44379</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="32"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="39">
+        <v>44379</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="32"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="33"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="34"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="28"/>
+      <c r="C35" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="35"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+    </row>
+    <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>1</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>2</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>3</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>4</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="10"/>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>5</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="10"/>
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>6</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="10"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="14">
+        <v>7</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="15"/>
+      <c r="F44" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C12" r:id="rId1"/>
+    <hyperlink ref="C38" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
TC03_ProductsTest TC04_ProductsTest Manual Test cases is added
</commit_message>
<xml_diff>
--- a/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
+++ b/InvoiceNinja/src/main/resources/ManualTestCaseDoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19380" windowHeight="6510" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14835" windowHeight="6510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -518,6 +518,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1061,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A18:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,17 +1324,11 @@
       <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
     </row>
-    <row r="60" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="9"/>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D60" s="6"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
@@ -1442,49 +1439,69 @@
       <c r="E69" s="36"/>
       <c r="F69" s="36"/>
     </row>
-    <row r="70" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="9"/>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D70" s="6"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
+      <c r="A71" s="17"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
       <c r="D71" s="6"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="6"/>
+    <row r="72" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="D72" s="6"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
+      <c r="B73" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
+      <c r="B74" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C74" s="6"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
-      <c r="B75" s="13"/>
+      <c r="B75" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
@@ -1492,22 +1509,20 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
-      <c r="B76" s="7"/>
+      <c r="B76" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A77" s="5"/>
+      <c r="B77" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C77" s="5"/>
       <c r="D77" s="3" t="s">
         <v>14</v>
       </c>
@@ -1518,24 +1533,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="17"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
+    <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+      <c r="B78" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C78" s="5"/>
       <c r="D78" s="17"/>
       <c r="E78" s="17"/>
       <c r="F78" s="17"/>
     </row>
-    <row r="79" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>25</v>
-      </c>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="14"/>
+      <c r="B79" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C79" s="14"/>
       <c r="D79" s="6" t="s">
         <v>23</v>
       </c>
@@ -1543,95 +1556,58 @@
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-      <c r="B80" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="A80" s="45"/>
+      <c r="B80" s="45"/>
+      <c r="C80" s="45"/>
       <c r="D80" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
     </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C81" s="6"/>
+    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D81" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C82" s="5"/>
+    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D82" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-      <c r="B83" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C83" s="5"/>
+    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D83" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
     </row>
-    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-      <c r="B84" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C84" s="5"/>
+    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D84" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
     </row>
-    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-      <c r="B85" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C85" s="5"/>
+    <row r="85" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D85" s="6" t="s">
         <v>35</v>
       </c>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
-      <c r="B86" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C86" s="14"/>
+    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D86" s="16" t="s">
         <v>23</v>
       </c>
       <c r="E86" s="14"/>
       <c r="F86" s="14"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="17"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="17"/>
+    <row r="87" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D87" s="17"/>
       <c r="E87" s="17"/>
       <c r="F87" s="17"/>

</xml_diff>